<commit_message>
second step to import from robohelp
</commit_message>
<xml_diff>
--- a/Table of Contents.report.xlsx
+++ b/Table of Contents.report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\saberprojects\kasra\kasra-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F2C4A8-2922-445D-815C-B8455B3188D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{369E137E-C193-4B5A-A98F-5AC5632BFA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{B4C4152B-3F25-43B2-B9B8-48547414F52A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6172" uniqueCount="1676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6172" uniqueCount="1677">
   <si>
     <t>Title</t>
   </si>
@@ -5066,6 +5066,9 @@
   </si>
   <si>
     <t>microcontent</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -5710,7 +5713,7 @@
   <autoFilter ref="A1:F942" xr:uid="{D4B95774-D85D-48BA-8979-EC9B64CDE414}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B193BF8A-7468-410A-96B9-03607011C987}" name="Title"/>
-    <tableColumn id="2" xr3:uid="{1EA13966-8AC0-4F7A-957F-C918FEA5136E}" name=" Reference"/>
+    <tableColumn id="2" xr3:uid="{1EA13966-8AC0-4F7A-957F-C918FEA5136E}" name="Reference"/>
     <tableColumn id="3" xr3:uid="{6F16196B-2079-4D50-9CB5-89FEF1846CDB}" name="Persian"/>
     <tableColumn id="4" xr3:uid="{616E6F81-DA45-4637-8551-860E37C4BF94}" name=" Type"/>
     <tableColumn id="5" xr3:uid="{984249F0-D0E7-465C-A700-B130887F93C9}" name=" Hidden"/>
@@ -6057,7 +6060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D388A7-6F02-401A-9892-1AFE90BEB072}">
   <dimension ref="A1:F278"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A186" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10814,13 +10817,13 @@
   <dimension ref="A1:F942"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
@@ -10831,7 +10834,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>1676</v>
       </c>
       <c r="C1" t="s">
         <v>1021</v>
@@ -26855,7 +26858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3268A1-4E4A-4DBA-973F-0BC3C69DF660}">
   <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A200" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>